<commit_message>
Prodigi & Proaktif proses done
</commit_message>
<xml_diff>
--- a/BA.xlsx
+++ b/BA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\prodigi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39BD43FC-AA8B-40F1-AEAC-7A1C156BD109}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C40FEC-4F49-4B3A-9D9B-F9A07AB359E6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="20490" windowHeight="7530" tabRatio="845"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="20490" windowHeight="7530" tabRatio="845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BA" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>PT. MEDIA MUSIK PROAKTIF</t>
   </si>
@@ -73,9 +73,6 @@
     <t>RBT Payment For Artis</t>
   </si>
   <si>
-    <t>Jan'17 - Dec'17</t>
-  </si>
-  <si>
     <t>Maka dengan ini kami memberitahukan bahwa pembayaran adalah sebesar</t>
   </si>
   <si>
@@ -109,11 +106,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$Rp-421]* #,##0_);_([$Rp-421]* \(#,##0\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$Rp-421]* #,##0.00_);_([$Rp-421]* \(#,##0.00\);_([$Rp-421]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -493,7 +490,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -517,6 +514,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -556,19 +554,18 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Comma 2" xfId="1"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="2"/>
-    <cellStyle name="Normal 11" xfId="3"/>
-    <cellStyle name="Normal 12" xfId="4"/>
-    <cellStyle name="Normal 15" xfId="5"/>
-    <cellStyle name="Normal 19" xfId="6"/>
-    <cellStyle name="Normal 20" xfId="7"/>
-    <cellStyle name="Normal 3" xfId="8"/>
-    <cellStyle name="Normal 5" xfId="9"/>
+    <cellStyle name="Normal 10" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 11" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 12" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 15" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 19" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 20" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -903,11 +900,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:V154"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,9 +1073,7 @@
       <c r="E11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -1113,7 +1108,7 @@
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>8</v>
@@ -1132,11 +1127,11 @@
     <row r="14" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="31"/>
       <c r="I14" s="17" t="s">
         <v>10</v>
       </c>
@@ -1150,15 +1145,15 @@
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="32" t="s">
-        <v>23</v>
+      <c r="D15" s="33" t="s">
+        <v>22</v>
       </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
       <c r="G15" s="5"/>
       <c r="H15" s="21"/>
       <c r="I15" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J15" s="19"/>
       <c r="K15" s="2"/>
@@ -1169,15 +1164,15 @@
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="32" t="s">
-        <v>24</v>
+      <c r="D16" s="33" t="s">
+        <v>23</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="5"/>
       <c r="H16" s="21"/>
       <c r="I16" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J16" s="19"/>
       <c r="K16" s="2"/>
@@ -1189,14 +1184,14 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="28"/>
       <c r="G17" s="5"/>
       <c r="H17" s="21"/>
-      <c r="I17" s="42" t="s">
-        <v>20</v>
+      <c r="I17" s="29" t="s">
+        <v>19</v>
       </c>
       <c r="J17" s="19"/>
       <c r="K17" s="2"/>
@@ -1207,15 +1202,15 @@
     <row r="18" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="32" t="s">
-        <v>26</v>
+      <c r="D18" s="33" t="s">
+        <v>25</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="5"/>
       <c r="H18" s="21"/>
       <c r="I18" s="24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J18" s="19"/>
       <c r="K18" s="2"/>
@@ -1226,11 +1221,11 @@
     <row r="19" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="6"/>
       <c r="J19" s="20"/>
       <c r="K19" s="2"/>
@@ -1257,7 +1252,7 @@
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B21" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -1266,7 +1261,7 @@
       <c r="G21" s="16"/>
       <c r="H21" s="16"/>
       <c r="I21" s="25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
@@ -1283,29 +1278,29 @@
       <c r="V21" s="7"/>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="N22" s="36"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="36"/>
-      <c r="Q22" s="36"/>
-      <c r="R22" s="36"/>
-      <c r="S22" s="36"/>
-      <c r="T22" s="36"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="36"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="37"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
@@ -1331,19 +1326,19 @@
       <c r="V23" s="7"/>
     </row>
     <row r="24" spans="2:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
@@ -1373,7 +1368,7 @@
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1447,10 +1442,10 @@
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
-      <c r="I30" s="35" t="s">
+      <c r="I30" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="J30" s="35"/>
+      <c r="J30" s="36"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>

</xml_diff>